<commit_message>
[Doc] Commit các file doc của report
Commit các file Q&A, file dịch các progress report
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/My coding tasks.xlsx
+++ b/WIP/Users/HuyenPT/My coding tasks.xlsx
@@ -115,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +174,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -186,6 +192,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -566,7 +575,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Coding]_Update post trong group
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/My coding tasks.xlsx
+++ b/WIP/Users/HuyenPT/My coding tasks.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>CÁC PHẦN CÒN LẠI CẦN ĐƯỢC UPDATE</t>
   </si>
@@ -79,6 +78,67 @@
   </si>
   <si>
     <t>Khi ấn edit, lấy id của bài post để làm id cho pop-up</t>
+  </si>
+  <si>
+    <t>all client load post</t>
+  </si>
+  <si>
+    <t>hoi Nhien</t>
+  </si>
+  <si>
+    <t>delete cmt</t>
+  </si>
+  <si>
+    <t>bỏ</t>
+  </si>
+  <si>
+    <t>cách lầy lội của Đăng</t>
+  </si>
+  <si>
+    <t>Hiển thị avatar</t>
+  </si>
+  <si>
+    <t>Trang chủ</t>
+  </si>
+  <si>
+    <t>Edit lấy Id của bài post</t>
+  </si>
+  <si>
+    <t>Phương án A</t>
+  </si>
+  <si>
+    <t>Phương án B</t>
+  </si>
+  <si>
+    <t>layout-hub</t>
+  </si>
+  <si>
+    <t>Tag book</t>
+  </si>
+  <si>
+    <t>bắt buộc phải có</t>
+  </si>
+  <si>
+    <t>Ẩn nút sửa xóa bài post nếu ko phải owner</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Lấy groupId</t>
+  </si>
+  <si>
+    <t>Huyền fix</t>
+  </si>
+  <si>
+    <t>post null</t>
+  </si>
+  <si>
+    <t>Đăng thử đến 5h</t>
+  </si>
+  <si>
+    <t>đổi trạng thái 
+thích - đã thích - bỏ thích</t>
   </si>
 </sst>
 </file>
@@ -115,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +201,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +252,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -190,11 +268,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -499,9 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E22"/>
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -510,11 +600,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -522,7 +612,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -575,7 +665,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -588,7 +678,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -608,6 +698,14 @@
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E22" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -621,24 +719,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>